<commit_message>
add util read data from excel
</commit_message>
<xml_diff>
--- a/ItemList.xlsx
+++ b/ItemList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="269">
   <si>
     <t>Safety</t>
   </si>
@@ -522,9 +522,6 @@
   </si>
   <si>
     <t>Steering wheel tilt/slide/lock</t>
-  </si>
-  <si>
-    <t>2 x Keys and or Fobs</t>
   </si>
   <si>
     <t>Heating &amp;amp; cooling performance check including heated seats</t>
@@ -869,7 +866,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:C262"/>
+  <dimension ref="B1:C261"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2317,15 +2314,15 @@
     </row>
     <row r="181">
       <c r="B181" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C181" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="182">
       <c r="B182" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C182" t="s">
         <v>187</v>
@@ -2333,7 +2330,7 @@
     </row>
     <row r="183">
       <c r="B183" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C183" t="s">
         <v>188</v>
@@ -2341,7 +2338,7 @@
     </row>
     <row r="184">
       <c r="B184" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C184" t="s">
         <v>189</v>
@@ -2349,7 +2346,7 @@
     </row>
     <row r="185">
       <c r="B185" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C185" t="s">
         <v>190</v>
@@ -2357,7 +2354,7 @@
     </row>
     <row r="186">
       <c r="B186" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C186" t="s">
         <v>191</v>
@@ -2365,7 +2362,7 @@
     </row>
     <row r="187">
       <c r="B187" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C187" t="s">
         <v>192</v>
@@ -2373,7 +2370,7 @@
     </row>
     <row r="188">
       <c r="B188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C188" t="s">
         <v>193</v>
@@ -2381,7 +2378,7 @@
     </row>
     <row r="189">
       <c r="B189" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C189" t="s">
         <v>194</v>
@@ -2389,7 +2386,7 @@
     </row>
     <row r="190">
       <c r="B190" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C190" t="s">
         <v>195</v>
@@ -2397,7 +2394,7 @@
     </row>
     <row r="191">
       <c r="B191" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C191" t="s">
         <v>196</v>
@@ -2405,7 +2402,7 @@
     </row>
     <row r="192">
       <c r="B192" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C192" t="s">
         <v>197</v>
@@ -2413,7 +2410,7 @@
     </row>
     <row r="193">
       <c r="B193" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C193" t="s">
         <v>198</v>
@@ -2421,7 +2418,7 @@
     </row>
     <row r="194">
       <c r="B194" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C194" t="s">
         <v>199</v>
@@ -2429,7 +2426,7 @@
     </row>
     <row r="195">
       <c r="B195" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C195" t="s">
         <v>200</v>
@@ -2437,7 +2434,7 @@
     </row>
     <row r="196">
       <c r="B196" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C196" t="s">
         <v>201</v>
@@ -2445,7 +2442,7 @@
     </row>
     <row r="197">
       <c r="B197" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C197" t="s">
         <v>202</v>
@@ -2453,7 +2450,7 @@
     </row>
     <row r="198">
       <c r="B198" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C198" t="s">
         <v>203</v>
@@ -2461,7 +2458,7 @@
     </row>
     <row r="199">
       <c r="B199" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C199" t="s">
         <v>204</v>
@@ -2469,7 +2466,7 @@
     </row>
     <row r="200">
       <c r="B200" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C200" t="s">
         <v>205</v>
@@ -2477,7 +2474,7 @@
     </row>
     <row r="201">
       <c r="B201" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C201" t="s">
         <v>206</v>
@@ -2485,7 +2482,7 @@
     </row>
     <row r="202">
       <c r="B202" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C202" t="s">
         <v>207</v>
@@ -2493,15 +2490,15 @@
     </row>
     <row r="203">
       <c r="B203" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="C203" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="204">
       <c r="B204" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C204" t="s">
         <v>210</v>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="205">
       <c r="B205" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C205" t="s">
         <v>211</v>
@@ -2517,7 +2514,7 @@
     </row>
     <row r="206">
       <c r="B206" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C206" t="s">
         <v>212</v>
@@ -2525,7 +2522,7 @@
     </row>
     <row r="207">
       <c r="B207" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C207" t="s">
         <v>213</v>
@@ -2533,7 +2530,7 @@
     </row>
     <row r="208">
       <c r="B208" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C208" t="s">
         <v>214</v>
@@ -2541,7 +2538,7 @@
     </row>
     <row r="209">
       <c r="B209" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C209" t="s">
         <v>215</v>
@@ -2549,7 +2546,7 @@
     </row>
     <row r="210">
       <c r="B210" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C210" t="s">
         <v>216</v>
@@ -2557,7 +2554,7 @@
     </row>
     <row r="211">
       <c r="B211" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C211" t="s">
         <v>217</v>
@@ -2565,7 +2562,7 @@
     </row>
     <row r="212">
       <c r="B212" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C212" t="s">
         <v>218</v>
@@ -2573,7 +2570,7 @@
     </row>
     <row r="213">
       <c r="B213" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C213" t="s">
         <v>219</v>
@@ -2581,7 +2578,7 @@
     </row>
     <row r="214">
       <c r="B214" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C214" t="s">
         <v>220</v>
@@ -2589,7 +2586,7 @@
     </row>
     <row r="215">
       <c r="B215" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C215" t="s">
         <v>221</v>
@@ -2597,7 +2594,7 @@
     </row>
     <row r="216">
       <c r="B216" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C216" t="s">
         <v>222</v>
@@ -2605,7 +2602,7 @@
     </row>
     <row r="217">
       <c r="B217" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C217" t="s">
         <v>223</v>
@@ -2613,7 +2610,7 @@
     </row>
     <row r="218">
       <c r="B218" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C218" t="s">
         <v>224</v>
@@ -2621,7 +2618,7 @@
     </row>
     <row r="219">
       <c r="B219" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C219" t="s">
         <v>225</v>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="220">
       <c r="B220" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C220" t="s">
         <v>226</v>
@@ -2637,7 +2634,7 @@
     </row>
     <row r="221">
       <c r="B221" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C221" t="s">
         <v>227</v>
@@ -2645,7 +2642,7 @@
     </row>
     <row r="222">
       <c r="B222" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C222" t="s">
         <v>228</v>
@@ -2653,7 +2650,7 @@
     </row>
     <row r="223">
       <c r="B223" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C223" t="s">
         <v>229</v>
@@ -2661,7 +2658,7 @@
     </row>
     <row r="224">
       <c r="B224" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C224" t="s">
         <v>230</v>
@@ -2669,7 +2666,7 @@
     </row>
     <row r="225">
       <c r="B225" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C225" t="s">
         <v>231</v>
@@ -2677,7 +2674,7 @@
     </row>
     <row r="226">
       <c r="B226" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C226" t="s">
         <v>232</v>
@@ -2685,7 +2682,7 @@
     </row>
     <row r="227">
       <c r="B227" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C227" t="s">
         <v>233</v>
@@ -2693,7 +2690,7 @@
     </row>
     <row r="228">
       <c r="B228" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C228" t="s">
         <v>234</v>
@@ -2701,7 +2698,7 @@
     </row>
     <row r="229">
       <c r="B229" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C229" t="s">
         <v>235</v>
@@ -2709,7 +2706,7 @@
     </row>
     <row r="230">
       <c r="B230" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C230" t="s">
         <v>236</v>
@@ -2717,7 +2714,7 @@
     </row>
     <row r="231">
       <c r="B231" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C231" t="s">
         <v>237</v>
@@ -2725,7 +2722,7 @@
     </row>
     <row r="232">
       <c r="B232" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C232" t="s">
         <v>238</v>
@@ -2733,7 +2730,7 @@
     </row>
     <row r="233">
       <c r="B233" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C233" t="s">
         <v>239</v>
@@ -2741,7 +2738,7 @@
     </row>
     <row r="234">
       <c r="B234" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C234" t="s">
         <v>240</v>
@@ -2749,7 +2746,7 @@
     </row>
     <row r="235">
       <c r="B235" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C235" t="s">
         <v>241</v>
@@ -2757,7 +2754,7 @@
     </row>
     <row r="236">
       <c r="B236" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C236" t="s">
         <v>242</v>
@@ -2765,7 +2762,7 @@
     </row>
     <row r="237">
       <c r="B237" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C237" t="s">
         <v>243</v>
@@ -2773,7 +2770,7 @@
     </row>
     <row r="238">
       <c r="B238" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C238" t="s">
         <v>244</v>
@@ -2781,7 +2778,7 @@
     </row>
     <row r="239">
       <c r="B239" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C239" t="s">
         <v>245</v>
@@ -2789,7 +2786,7 @@
     </row>
     <row r="240">
       <c r="B240" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C240" t="s">
         <v>246</v>
@@ -2797,7 +2794,7 @@
     </row>
     <row r="241">
       <c r="B241" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C241" t="s">
         <v>247</v>
@@ -2805,7 +2802,7 @@
     </row>
     <row r="242">
       <c r="B242" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C242" t="s">
         <v>248</v>
@@ -2813,7 +2810,7 @@
     </row>
     <row r="243">
       <c r="B243" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C243" t="s">
         <v>249</v>
@@ -2821,7 +2818,7 @@
     </row>
     <row r="244">
       <c r="B244" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C244" t="s">
         <v>250</v>
@@ -2829,7 +2826,7 @@
     </row>
     <row r="245">
       <c r="B245" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C245" t="s">
         <v>251</v>
@@ -2837,15 +2834,15 @@
     </row>
     <row r="246">
       <c r="B246" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
       <c r="C246" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="247">
       <c r="B247" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C247" t="s">
         <v>254</v>
@@ -2853,7 +2850,7 @@
     </row>
     <row r="248">
       <c r="B248" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C248" t="s">
         <v>255</v>
@@ -2861,7 +2858,7 @@
     </row>
     <row r="249">
       <c r="B249" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C249" t="s">
         <v>256</v>
@@ -2869,7 +2866,7 @@
     </row>
     <row r="250">
       <c r="B250" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C250" t="s">
         <v>257</v>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="251">
       <c r="B251" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C251" t="s">
         <v>258</v>
@@ -2885,7 +2882,7 @@
     </row>
     <row r="252">
       <c r="B252" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C252" t="s">
         <v>259</v>
@@ -2893,7 +2890,7 @@
     </row>
     <row r="253">
       <c r="B253" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C253" t="s">
         <v>260</v>
@@ -2901,7 +2898,7 @@
     </row>
     <row r="254">
       <c r="B254" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C254" t="s">
         <v>261</v>
@@ -2909,7 +2906,7 @@
     </row>
     <row r="255">
       <c r="B255" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C255" t="s">
         <v>262</v>
@@ -2917,7 +2914,7 @@
     </row>
     <row r="256">
       <c r="B256" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C256" t="s">
         <v>263</v>
@@ -2925,7 +2922,7 @@
     </row>
     <row r="257">
       <c r="B257" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C257" t="s">
         <v>264</v>
@@ -2933,7 +2930,7 @@
     </row>
     <row r="258">
       <c r="B258" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C258" t="s">
         <v>265</v>
@@ -2941,7 +2938,7 @@
     </row>
     <row r="259">
       <c r="B259" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C259" t="s">
         <v>266</v>
@@ -2949,7 +2946,7 @@
     </row>
     <row r="260">
       <c r="B260" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C260" t="s">
         <v>267</v>
@@ -2957,18 +2954,10 @@
     </row>
     <row r="261">
       <c r="B261" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C261" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="B262" t="s">
-        <v>253</v>
-      </c>
-      <c r="C262" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>